<commit_message>
add plywood to estimate
</commit_message>
<xml_diff>
--- a/doc/fab_estimate.xlsx
+++ b/doc/fab_estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\braille\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1673D09E-CE68-4A28-AE43-E5F635004B36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826EB7F-4F80-42A3-B876-9A6D80EEB1AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="890" yWindow="0" windowWidth="8830" windowHeight="5930" xr2:uid="{C8CFA7FD-6112-441E-9599-86EC42024663}"/>
+    <workbookView xWindow="1780" yWindow="0" windowWidth="8830" windowHeight="5930" xr2:uid="{C8CFA7FD-6112-441E-9599-86EC42024663}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Кол-во</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Кабель mini-USB-BM USB-AM F</t>
+  </si>
+  <si>
+    <t>фанера ФК сорт 2/4 1525х1525х4мм</t>
+  </si>
+  <si>
+    <t>https://www.maxidom.ru/catalog/fanera/1001088706/</t>
   </si>
 </sst>
 </file>
@@ -621,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0409B55-D371-47F8-8BCE-3990C9654127}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -710,7 +716,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G7" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G8" si="0">E4*F4</f>
         <v>120</v>
       </c>
       <c r="H4" s="8"/>
@@ -795,49 +801,74 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>487</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>487</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>225</v>
       </c>
-      <c r="G8" s="2">
-        <f>E8*F8</f>
+      <c r="G9" s="2">
+        <f>E9*F9</f>
         <v>900</v>
       </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9" t="s">
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11">
-        <f>SUM(G3:G8)</f>
-        <v>1695</v>
-      </c>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E13" s="1"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11">
+        <f>SUM(G3:G9)</f>
+        <v>2182</v>
+      </c>
+      <c r="H10" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>